<commit_message>
Filtro por estado, imagens
</commit_message>
<xml_diff>
--- a/Recomendacoes/campanhas.xlsx
+++ b/Recomendacoes/campanhas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evilj\hortasync\Recomendacoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0252DE-1B37-428E-9468-D40286A1CE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D438457A-1289-4FD1-A0CF-ABF81E7B7918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14730" yWindow="4410" windowWidth="19620" windowHeight="10050" xr2:uid="{895F0F17-1DC9-41D5-8D72-F1595099C9CF}"/>
+    <workbookView xWindow="-270" yWindow="3600" windowWidth="25770" windowHeight="10050" xr2:uid="{895F0F17-1DC9-41D5-8D72-F1595099C9CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -233,9 +233,6 @@
     <t>ferramentas,equipamento, enxada</t>
   </si>
   <si>
-    <t>matterial,ferramentas</t>
-  </si>
-  <si>
     <t>solo,adubo</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>Imagens/Hortas/mudasdearvore.png</t>
   </si>
   <si>
-    <t>Imagens/Hortas/Irrigacao.jpg'</t>
-  </si>
-  <si>
     <t>Imagens/Hortas/sensoresdeumidade.jpg</t>
   </si>
   <si>
@@ -342,6 +336,12 @@
   </si>
   <si>
     <t>imagem</t>
+  </si>
+  <si>
+    <t>Imagens/Hortas/Irrigacao.jpg</t>
+  </si>
+  <si>
+    <t>material,ferramentas</t>
   </si>
 </sst>
 </file>
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCA1DF9-033E-47B6-A790-9A3615843AD9}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +819,7 @@
         <v>15</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>16</v>
@@ -857,7 +857,7 @@
         <v>10000</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L2" s="1">
         <v>45332</v>
@@ -883,7 +883,7 @@
         <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="H3">
         <v>4500</v>
@@ -895,7 +895,7 @@
         <v>12000</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L3" s="1">
         <v>45342</v>
@@ -933,7 +933,7 @@
         <v>5000</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L4" s="1">
         <v>45349</v>
@@ -971,7 +971,7 @@
         <v>4000</v>
       </c>
       <c r="K5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L5" s="1">
         <v>45338</v>
@@ -1009,7 +1009,7 @@
         <v>8000</v>
       </c>
       <c r="K6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L6" s="1">
         <v>45350</v>
@@ -1035,7 +1035,7 @@
         <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H7">
         <v>211</v>
@@ -1047,7 +1047,7 @@
         <v>9000</v>
       </c>
       <c r="K7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L7" s="1">
         <v>45348</v>
@@ -1073,7 +1073,7 @@
         <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H8">
         <v>545</v>
@@ -1085,7 +1085,7 @@
         <v>11500</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L8" s="1">
         <v>45348</v>
@@ -1111,7 +1111,7 @@
         <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H9">
         <v>3200</v>
@@ -1123,7 +1123,7 @@
         <v>9000</v>
       </c>
       <c r="K9" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="L9" s="1">
         <v>45337</v>
@@ -1149,7 +1149,7 @@
         <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H10">
         <v>700</v>
@@ -1161,7 +1161,7 @@
         <v>10000</v>
       </c>
       <c r="K10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L10" s="1">
         <v>45347</v>
@@ -1187,7 +1187,7 @@
         <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H11">
         <v>800</v>
@@ -1199,7 +1199,7 @@
         <v>7000</v>
       </c>
       <c r="K11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L11" s="1">
         <v>45345</v>
@@ -1225,7 +1225,7 @@
         <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H12">
         <v>400</v>
@@ -1237,7 +1237,7 @@
         <v>11000</v>
       </c>
       <c r="K12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L12" s="1">
         <v>45337</v>
@@ -1263,7 +1263,7 @@
         <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H13">
         <v>761</v>
@@ -1275,7 +1275,7 @@
         <v>8000</v>
       </c>
       <c r="K13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L13" s="1">
         <v>45332</v>
@@ -1301,7 +1301,7 @@
         <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H14">
         <v>3488</v>
@@ -1313,7 +1313,7 @@
         <v>15000</v>
       </c>
       <c r="K14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L14" s="1">
         <v>45351</v>
@@ -1339,7 +1339,7 @@
         <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H15">
         <v>354</v>
@@ -1351,7 +1351,7 @@
         <v>7500</v>
       </c>
       <c r="K15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L15" s="1">
         <v>45352</v>
@@ -1377,7 +1377,7 @@
         <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H16">
         <v>876</v>
@@ -1389,7 +1389,7 @@
         <v>10000</v>
       </c>
       <c r="K16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L16" s="1">
         <v>45341</v>
@@ -1415,7 +1415,7 @@
         <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H17">
         <v>788</v>
@@ -1427,7 +1427,7 @@
         <v>8000</v>
       </c>
       <c r="K17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L17" s="1">
         <v>45350</v>
@@ -1453,7 +1453,7 @@
         <v>36</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H18">
         <v>767</v>
@@ -1465,7 +1465,7 @@
         <v>9000</v>
       </c>
       <c r="K18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L18" s="1">
         <v>45352</v>
@@ -1491,7 +1491,7 @@
         <v>32</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H19">
         <v>325</v>
@@ -1503,7 +1503,7 @@
         <v>14500</v>
       </c>
       <c r="K19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L19" s="1">
         <v>45371</v>
@@ -1514,7 +1514,7 @@
         <v>357</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1529,7 +1529,7 @@
         <v>32</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H20">
         <v>2555</v>
@@ -1541,7 +1541,7 @@
         <v>7000</v>
       </c>
       <c r="K20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L20" s="1">
         <v>45350</v>
@@ -1567,7 +1567,7 @@
         <v>34</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H21">
         <v>4589</v>
@@ -1579,7 +1579,7 @@
         <v>4800</v>
       </c>
       <c r="K21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L21" s="1">
         <v>45332</v>
@@ -1605,7 +1605,7 @@
         <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H22">
         <v>767</v>
@@ -1617,7 +1617,7 @@
         <v>3800</v>
       </c>
       <c r="K22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L22" s="1">
         <v>45341</v>

</xml_diff>